<commit_message>
updated test case status and MnS in report packing
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesSystemTest_LPH.xlsx
+++ b/Library/excelTestCasesSystemTest_LPH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20484" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="21420" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>Billing\OPbilling\TC008BillingSaleDepositDeductPlusTenderCashReturn.py</t>
   </si>
   <si>
-    <t>Billing\OPbilling\TC009CreateProvisionalBill.py</t>
-  </si>
-  <si>
     <t>Billing\OPbilling\TC011CreateCopyOfItemsCashInvoice.py</t>
   </si>
   <si>
@@ -391,6 +388,9 @@
   </si>
   <si>
     <t>Norun</t>
+  </si>
+  <si>
+    <t>Billing\OPbilling\TC009CreateEstimationBill.py</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,10 +790,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>82</v>
@@ -802,7 +802,7 @@
         <v>84</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -850,7 +850,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -870,7 +870,7 @@
         <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -890,7 +890,7 @@
         <v>88</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -910,7 +910,7 @@
         <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -930,7 +930,7 @@
         <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -950,7 +950,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -1007,10 +1007,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -1027,10 +1027,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -1050,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -1070,7 +1070,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -1090,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1110,7 +1110,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1130,7 +1130,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1150,7 +1150,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1170,7 +1170,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -1190,7 +1190,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1210,7 +1210,7 @@
         <v>35</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1230,7 +1230,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1250,7 +1250,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1270,7 +1270,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1290,7 +1290,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -1310,7 +1310,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1330,7 +1330,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1350,7 +1350,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1370,7 +1370,7 @@
         <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1390,7 +1390,7 @@
         <v>53</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1410,7 +1410,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -1447,10 +1447,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -1467,10 +1467,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -1490,7 +1490,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1510,7 +1510,7 @@
         <v>60</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1530,7 +1530,7 @@
         <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -1550,7 +1550,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -1570,7 +1570,7 @@
         <v>66</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -1590,7 +1590,7 @@
         <v>68</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -1610,7 +1610,7 @@
         <v>70</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -1630,7 +1630,7 @@
         <v>72</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1650,7 +1650,7 @@
         <v>74</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -1670,7 +1670,7 @@
         <v>76</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -1690,7 +1690,7 @@
         <v>78</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -1710,7 +1710,7 @@
         <v>80</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -1730,7 +1730,7 @@
         <v>83</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1747,10 +1747,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>4</v>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1767,10 +1767,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>4</v>
@@ -1779,7 +1779,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1787,10 +1787,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>4</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1807,10 +1807,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>4</v>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -1827,10 +1827,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>4</v>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>4</v>
@@ -1859,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>4</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1887,10 +1887,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>4</v>
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -1907,10 +1907,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>4</v>
@@ -1919,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -1927,10 +1927,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>4</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>

</xml_diff>